<commit_message>
Red and Purple size/Density plots added
</commit_message>
<xml_diff>
--- a/data/density_experiment/derived/urchin_density_data_cleaned.xlsx
+++ b/data/density_experiment/derived/urchin_density_data_cleaned.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maerennick/GitHub/Rennick-2019-urchin-grazing/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maerennick/GitHub/Rennick-2019-urchin-grazing/data/density_experiment/derived/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1996354-17F9-5F49-A5CA-977F67D935DF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1626E758-FC5B-694C-BFAC-EB18A93F7B19}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="27640" windowHeight="16100" xr2:uid="{BE3A720F-A9A8-7C4C-A632-649EFD71C71F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27640" windowHeight="16100" xr2:uid="{BE3A720F-A9A8-7C4C-A632-649EFD71C71F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="urchin_density_data_cleaned" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">urchin_density_data_cleaned!$A$1:$M$619</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -698,10 +701,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C72C63-6C19-3643-86E3-FB14F76C4933}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:M619"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A411" zoomScale="109" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:B597"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -747,7 +751,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43649</v>
       </c>
@@ -786,7 +790,7 @@
         <v>223.7</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43649</v>
       </c>
@@ -825,7 +829,7 @@
         <v>223.7</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43649</v>
       </c>
@@ -864,7 +868,7 @@
         <v>223.7</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43649</v>
       </c>
@@ -903,7 +907,7 @@
         <v>223.7</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43649</v>
       </c>
@@ -942,7 +946,7 @@
         <v>223.7</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43649</v>
       </c>
@@ -981,7 +985,7 @@
         <v>223.7</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43649</v>
       </c>
@@ -1332,7 +1336,7 @@
         <v>183.1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43649</v>
       </c>
@@ -1371,7 +1375,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43649</v>
       </c>
@@ -1410,7 +1414,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43649</v>
       </c>
@@ -1449,7 +1453,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43649</v>
       </c>
@@ -1488,7 +1492,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43649</v>
       </c>
@@ -1527,7 +1531,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43649</v>
       </c>
@@ -1566,7 +1570,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43649</v>
       </c>
@@ -1605,7 +1609,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43649</v>
       </c>
@@ -1644,7 +1648,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43649</v>
       </c>
@@ -1683,7 +1687,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43649</v>
       </c>
@@ -1722,7 +1726,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43649</v>
       </c>
@@ -1761,7 +1765,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43649</v>
       </c>
@@ -1800,7 +1804,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43649</v>
       </c>
@@ -1839,7 +1843,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43649</v>
       </c>
@@ -1878,7 +1882,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43649</v>
       </c>
@@ -1917,7 +1921,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43649</v>
       </c>
@@ -1956,7 +1960,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43649</v>
       </c>
@@ -1995,7 +1999,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43649</v>
       </c>
@@ -2034,7 +2038,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43649</v>
       </c>
@@ -2073,7 +2077,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43649</v>
       </c>
@@ -2112,7 +2116,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43649</v>
       </c>
@@ -2151,7 +2155,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43649</v>
       </c>
@@ -2190,7 +2194,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43649</v>
       </c>
@@ -2229,7 +2233,7 @@
         <v>229.6</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43649</v>
       </c>
@@ -2268,7 +2272,7 @@
         <v>229.6</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>43649</v>
       </c>
@@ -2307,7 +2311,7 @@
         <v>229.6</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>43649</v>
       </c>
@@ -2346,7 +2350,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>43649</v>
       </c>
@@ -2385,7 +2389,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43649</v>
       </c>
@@ -2424,7 +2428,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43649</v>
       </c>
@@ -2463,7 +2467,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>43649</v>
       </c>
@@ -2502,7 +2506,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>43649</v>
       </c>
@@ -2541,7 +2545,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>43649</v>
       </c>
@@ -2580,7 +2584,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>43649</v>
       </c>
@@ -2619,7 +2623,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>43649</v>
       </c>
@@ -2658,7 +2662,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>43649</v>
       </c>
@@ -2697,7 +2701,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43649</v>
       </c>
@@ -2736,7 +2740,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>43649</v>
       </c>
@@ -2775,7 +2779,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>43649</v>
       </c>
@@ -2814,7 +2818,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>43649</v>
       </c>
@@ -2853,7 +2857,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>43649</v>
       </c>
@@ -2892,7 +2896,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>43649</v>
       </c>
@@ -2931,7 +2935,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>43649</v>
       </c>
@@ -2970,7 +2974,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>43649</v>
       </c>
@@ -3009,7 +3013,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>43649</v>
       </c>
@@ -3048,7 +3052,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>43649</v>
       </c>
@@ -3087,7 +3091,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>43649</v>
       </c>
@@ -3126,7 +3130,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>43649</v>
       </c>
@@ -3165,7 +3169,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>43649</v>
       </c>
@@ -3204,7 +3208,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>43649</v>
       </c>
@@ -3243,7 +3247,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>43649</v>
       </c>
@@ -3282,7 +3286,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>43649</v>
       </c>
@@ -3321,7 +3325,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>43649</v>
       </c>
@@ -3360,7 +3364,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>43649</v>
       </c>
@@ -3399,7 +3403,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>43649</v>
       </c>
@@ -3438,7 +3442,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>43649</v>
       </c>
@@ -3477,7 +3481,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>43649</v>
       </c>
@@ -3516,7 +3520,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>43649</v>
       </c>
@@ -3555,7 +3559,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>43649</v>
       </c>
@@ -3594,7 +3598,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>43649</v>
       </c>
@@ -3633,7 +3637,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>43649</v>
       </c>
@@ -3672,7 +3676,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>43649</v>
       </c>
@@ -3711,7 +3715,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>43649</v>
       </c>
@@ -3750,7 +3754,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>43649</v>
       </c>
@@ -3789,7 +3793,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>43649</v>
       </c>
@@ -3828,7 +3832,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>43649</v>
       </c>
@@ -3867,7 +3871,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>43649</v>
       </c>
@@ -3906,7 +3910,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>43649</v>
       </c>
@@ -3945,7 +3949,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>43649</v>
       </c>
@@ -3984,7 +3988,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>43649</v>
       </c>
@@ -4491,7 +4495,7 @@
         <v>135.6</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>43649</v>
       </c>
@@ -4530,7 +4534,7 @@
         <v>243.1</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>43649</v>
       </c>
@@ -4569,7 +4573,7 @@
         <v>243.1</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>43649</v>
       </c>
@@ -4608,7 +4612,7 @@
         <v>243.1</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>43649</v>
       </c>
@@ -4647,7 +4651,7 @@
         <v>243.1</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>43649</v>
       </c>
@@ -4686,7 +4690,7 @@
         <v>243.1</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>43649</v>
       </c>
@@ -4725,7 +4729,7 @@
         <v>243.1</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>43649</v>
       </c>
@@ -4764,7 +4768,7 @@
         <v>243.1</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>43649</v>
       </c>
@@ -4803,7 +4807,7 @@
         <v>243.1</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>43649</v>
       </c>
@@ -4842,7 +4846,7 @@
         <v>243.1</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>43649</v>
       </c>
@@ -4881,7 +4885,7 @@
         <v>243.1</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>43649</v>
       </c>
@@ -4920,7 +4924,7 @@
         <v>243.1</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>43649</v>
       </c>
@@ -4959,7 +4963,7 @@
         <v>251.5</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>43649</v>
       </c>
@@ -5115,7 +5119,7 @@
         <v>220.9</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>43649</v>
       </c>
@@ -5154,7 +5158,7 @@
         <v>235.3</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>43649</v>
       </c>
@@ -5193,7 +5197,7 @@
         <v>235.3</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>43649</v>
       </c>
@@ -5232,7 +5236,7 @@
         <v>235.3</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>43649</v>
       </c>
@@ -5271,7 +5275,7 @@
         <v>235.3</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>43649</v>
       </c>
@@ -5310,7 +5314,7 @@
         <v>235.3</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>43649</v>
       </c>
@@ -5349,7 +5353,7 @@
         <v>235.3</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>43649</v>
       </c>
@@ -5388,7 +5392,7 @@
         <v>235.3</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>43649</v>
       </c>
@@ -5427,7 +5431,7 @@
         <v>246.89999999999998</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>43649</v>
       </c>
@@ -5466,7 +5470,7 @@
         <v>246.89999999999998</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>43649</v>
       </c>
@@ -5505,7 +5509,7 @@
         <v>246.89999999999998</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>43649</v>
       </c>
@@ -5544,7 +5548,7 @@
         <v>246.89999999999998</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>43649</v>
       </c>
@@ -5583,7 +5587,7 @@
         <v>246.89999999999998</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>43649</v>
       </c>
@@ -5622,7 +5626,7 @@
         <v>246.89999999999998</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>43649</v>
       </c>
@@ -5661,7 +5665,7 @@
         <v>246.89999999999998</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>43649</v>
       </c>
@@ -5700,7 +5704,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>43649</v>
       </c>
@@ -5739,7 +5743,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>43649</v>
       </c>
@@ -5778,7 +5782,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>43649</v>
       </c>
@@ -5817,7 +5821,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>43649</v>
       </c>
@@ -5856,7 +5860,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>43649</v>
       </c>
@@ -5895,7 +5899,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>43649</v>
       </c>
@@ -5934,7 +5938,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>43649</v>
       </c>
@@ -5973,7 +5977,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>43649</v>
       </c>
@@ -6012,7 +6016,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>43649</v>
       </c>
@@ -6051,7 +6055,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>43649</v>
       </c>
@@ -6090,7 +6094,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>43649</v>
       </c>
@@ -6129,7 +6133,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>43649</v>
       </c>
@@ -6168,7 +6172,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>43649</v>
       </c>
@@ -6207,7 +6211,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>43649</v>
       </c>
@@ -6246,7 +6250,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>43649</v>
       </c>
@@ -6285,7 +6289,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>43649</v>
       </c>
@@ -6324,7 +6328,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>43649</v>
       </c>
@@ -6363,7 +6367,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>43649</v>
       </c>
@@ -6402,7 +6406,7 @@
         <v>210.7</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>43649</v>
       </c>
@@ -6441,7 +6445,7 @@
         <v>252.39999999999998</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>43649</v>
       </c>
@@ -6480,7 +6484,7 @@
         <v>252.39999999999998</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>43649</v>
       </c>
@@ -6636,7 +6640,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>43649</v>
       </c>
@@ -6675,7 +6679,7 @@
         <v>218.4</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>43649</v>
       </c>
@@ -6714,7 +6718,7 @@
         <v>218.4</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>43649</v>
       </c>
@@ -6753,7 +6757,7 @@
         <v>218.4</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>43649</v>
       </c>
@@ -6792,7 +6796,7 @@
         <v>218.4</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>43649</v>
       </c>
@@ -6831,7 +6835,7 @@
         <v>218.4</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>43649</v>
       </c>
@@ -6870,7 +6874,7 @@
         <v>218.4</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>43649</v>
       </c>
@@ -6909,7 +6913,7 @@
         <v>218.4</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>43649</v>
       </c>
@@ -6948,7 +6952,7 @@
         <v>218.4</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>43649</v>
       </c>
@@ -6987,7 +6991,7 @@
         <v>218.4</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>43649</v>
       </c>
@@ -7026,7 +7030,7 @@
         <v>218.4</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>43649</v>
       </c>
@@ -7065,7 +7069,7 @@
         <v>218.4</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>43649</v>
       </c>
@@ -7104,7 +7108,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>43649</v>
       </c>
@@ -7143,7 +7147,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>43649</v>
       </c>
@@ -7182,7 +7186,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>43649</v>
       </c>
@@ -7221,7 +7225,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>43649</v>
       </c>
@@ -7260,7 +7264,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>43649</v>
       </c>
@@ -7299,7 +7303,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>43649</v>
       </c>
@@ -7338,7 +7342,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>43649</v>
       </c>
@@ -7377,7 +7381,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>43649</v>
       </c>
@@ -7416,7 +7420,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>43649</v>
       </c>
@@ -7455,7 +7459,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>43649</v>
       </c>
@@ -7494,7 +7498,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>43649</v>
       </c>
@@ -7533,7 +7537,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>43649</v>
       </c>
@@ -7572,7 +7576,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>43649</v>
       </c>
@@ -7611,7 +7615,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>43649</v>
       </c>
@@ -7650,7 +7654,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>43649</v>
       </c>
@@ -7689,7 +7693,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>43649</v>
       </c>
@@ -7728,7 +7732,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>43649</v>
       </c>
@@ -7767,7 +7771,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>43649</v>
       </c>
@@ -7806,7 +7810,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>43649</v>
       </c>
@@ -7845,7 +7849,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>43649</v>
       </c>
@@ -7884,7 +7888,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>43649</v>
       </c>
@@ -7923,7 +7927,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>43649</v>
       </c>
@@ -7962,7 +7966,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>43649</v>
       </c>
@@ -8001,7 +8005,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>43649</v>
       </c>
@@ -8040,7 +8044,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>43649</v>
       </c>
@@ -8079,7 +8083,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>43649</v>
       </c>
@@ -8118,7 +8122,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>43649</v>
       </c>
@@ -8157,7 +8161,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>43649</v>
       </c>
@@ -8196,7 +8200,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>43649</v>
       </c>
@@ -8235,7 +8239,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>43649</v>
       </c>
@@ -8274,7 +8278,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>43649</v>
       </c>
@@ -8313,7 +8317,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>43649</v>
       </c>
@@ -8352,7 +8356,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>43649</v>
       </c>
@@ -8391,7 +8395,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>43649</v>
       </c>
@@ -8430,7 +8434,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>43649</v>
       </c>
@@ -8469,7 +8473,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>43649</v>
       </c>
@@ -8508,7 +8512,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>43649</v>
       </c>
@@ -8547,7 +8551,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>43649</v>
       </c>
@@ -8586,7 +8590,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>43649</v>
       </c>
@@ -8625,7 +8629,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>43649</v>
       </c>
@@ -8664,7 +8668,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>43649</v>
       </c>
@@ -8703,7 +8707,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>43649</v>
       </c>
@@ -8742,7 +8746,7 @@
         <v>159.80000000000001</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>43649</v>
       </c>
@@ -8859,7 +8863,7 @@
         <v>246.2</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>43649</v>
       </c>
@@ -8898,7 +8902,7 @@
         <v>244.7</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>43649</v>
       </c>
@@ -9005,17 +9009,17 @@
         <v>239</v>
       </c>
       <c r="J213">
-        <f>48-((17+(45/60))-(14+(37/60)))</f>
-        <v>44.866666666666667</v>
+        <f>(48*2)-((17+(45/60))-(13+(34/60)))</f>
+        <v>91.816666666666663</v>
       </c>
       <c r="K213">
         <v>250.4</v>
       </c>
       <c r="L213">
-        <v>253.2</v>
-      </c>
-    </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>43649</v>
       </c>
@@ -9054,7 +9058,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>43649</v>
       </c>
@@ -9093,7 +9097,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>43649</v>
       </c>
@@ -9132,7 +9136,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>43649</v>
       </c>
@@ -9171,7 +9175,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>43649</v>
       </c>
@@ -9210,7 +9214,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>43649</v>
       </c>
@@ -9249,7 +9253,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>43649</v>
       </c>
@@ -9288,7 +9292,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>43649</v>
       </c>
@@ -9327,7 +9331,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>43649</v>
       </c>
@@ -9366,7 +9370,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>43649</v>
       </c>
@@ -9405,7 +9409,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>43649</v>
       </c>
@@ -9444,7 +9448,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>43649</v>
       </c>
@@ -9483,7 +9487,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>43649</v>
       </c>
@@ -9522,7 +9526,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>43649</v>
       </c>
@@ -9561,7 +9565,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>43649</v>
       </c>
@@ -9600,7 +9604,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>43649</v>
       </c>
@@ -9639,7 +9643,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>43649</v>
       </c>
@@ -9678,7 +9682,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>43649</v>
       </c>
@@ -9717,7 +9721,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>43649</v>
       </c>
@@ -9756,7 +9760,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>43649</v>
       </c>
@@ -9795,7 +9799,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>43649</v>
       </c>
@@ -9834,7 +9838,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>43649</v>
       </c>
@@ -9873,7 +9877,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>43649</v>
       </c>
@@ -9912,7 +9916,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>43649</v>
       </c>
@@ -10224,7 +10228,7 @@
         <v>244.9</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>43649</v>
       </c>
@@ -10263,7 +10267,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>43649</v>
       </c>
@@ -10302,7 +10306,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>43649</v>
       </c>
@@ -10341,7 +10345,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>43649</v>
       </c>
@@ -10380,7 +10384,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>43649</v>
       </c>
@@ -10419,7 +10423,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>43649</v>
       </c>
@@ -10458,7 +10462,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>43649</v>
       </c>
@@ -10497,7 +10501,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>43649</v>
       </c>
@@ -10536,7 +10540,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>43649</v>
       </c>
@@ -10575,7 +10579,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>43649</v>
       </c>
@@ -10614,7 +10618,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>43649</v>
       </c>
@@ -10653,7 +10657,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>43649</v>
       </c>
@@ -10692,7 +10696,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>43649</v>
       </c>
@@ -10731,7 +10735,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>43649</v>
       </c>
@@ -10770,7 +10774,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>43649</v>
       </c>
@@ -10809,7 +10813,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>43649</v>
       </c>
@@ -10848,7 +10852,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>43649</v>
       </c>
@@ -10887,7 +10891,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>43649</v>
       </c>
@@ -10926,7 +10930,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>43649</v>
       </c>
@@ -10965,7 +10969,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>43649</v>
       </c>
@@ -11004,7 +11008,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>43649</v>
       </c>
@@ -11043,7 +11047,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>43649</v>
       </c>
@@ -11082,7 +11086,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>43649</v>
       </c>
@@ -11121,7 +11125,7 @@
         <v>200.6</v>
       </c>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>43649</v>
       </c>
@@ -11199,7 +11203,7 @@
         <v>243.1</v>
       </c>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>43649</v>
       </c>
@@ -11238,7 +11242,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>43649</v>
       </c>
@@ -11277,7 +11281,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>43649</v>
       </c>
@@ -11316,7 +11320,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>43649</v>
       </c>
@@ -11355,7 +11359,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>43649</v>
       </c>
@@ -11394,7 +11398,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>43649</v>
       </c>
@@ -11433,7 +11437,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>43649</v>
       </c>
@@ -11472,7 +11476,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>43649</v>
       </c>
@@ -11511,7 +11515,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>43649</v>
       </c>
@@ -11550,7 +11554,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
         <v>43649</v>
       </c>
@@ -11589,7 +11593,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>43649</v>
       </c>
@@ -11628,7 +11632,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>43649</v>
       </c>
@@ -11667,7 +11671,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
         <v>43649</v>
       </c>
@@ -11706,7 +11710,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" s="1">
         <v>43649</v>
       </c>
@@ -11745,7 +11749,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" s="1">
         <v>43649</v>
       </c>
@@ -11784,7 +11788,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>43649</v>
       </c>
@@ -11823,7 +11827,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
         <v>43649</v>
       </c>
@@ -11862,7 +11866,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" s="1">
         <v>43649</v>
       </c>
@@ -11901,7 +11905,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" s="1">
         <v>43649</v>
       </c>
@@ -11940,7 +11944,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" s="1">
         <v>43649</v>
       </c>
@@ -11979,7 +11983,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="290" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" s="1">
         <v>43649</v>
       </c>
@@ -12018,7 +12022,7 @@
         <v>200.1</v>
       </c>
     </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291" s="1">
         <v>43649</v>
       </c>
@@ -12525,7 +12529,7 @@
         <v>229.8</v>
       </c>
     </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304" s="1">
         <v>43649</v>
       </c>
@@ -12567,7 +12571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305" s="1">
         <v>43649</v>
       </c>
@@ -12609,7 +12613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A306" s="1">
         <v>43649</v>
       </c>
@@ -12651,7 +12655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A307" s="1">
         <v>43649</v>
       </c>
@@ -12693,7 +12697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A308" s="1">
         <v>43649</v>
       </c>
@@ -12735,7 +12739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A309" s="1">
         <v>43649</v>
       </c>
@@ -12777,7 +12781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A310" s="1">
         <v>43649</v>
       </c>
@@ -12819,7 +12823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A311" s="1">
         <v>43649</v>
       </c>
@@ -12861,7 +12865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A312" s="1">
         <v>43649</v>
       </c>
@@ -12903,7 +12907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313" s="1">
         <v>43649</v>
       </c>
@@ -12945,7 +12949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314" s="1">
         <v>43649</v>
       </c>
@@ -12987,7 +12991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315" s="1">
         <v>43649</v>
       </c>
@@ -13029,7 +13033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A316" s="1">
         <v>43649</v>
       </c>
@@ -13071,7 +13075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A317" s="1">
         <v>43649</v>
       </c>
@@ -13113,7 +13117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A318" s="1">
         <v>43649</v>
       </c>
@@ -13155,7 +13159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
         <v>43649</v>
       </c>
@@ -13197,7 +13201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320" s="1">
         <v>43649</v>
       </c>
@@ -13239,7 +13243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A321" s="1">
         <v>43649</v>
       </c>
@@ -13281,7 +13285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A322" s="1">
         <v>43649</v>
       </c>
@@ -13323,7 +13327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A323" s="1">
         <v>43649</v>
       </c>
@@ -13365,7 +13369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A324" s="1">
         <v>43649</v>
       </c>
@@ -13407,7 +13411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A325" s="1">
         <v>43649</v>
       </c>
@@ -13449,7 +13453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A326" s="1">
         <v>43649</v>
       </c>
@@ -13491,7 +13495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A327" s="1">
         <v>43649</v>
       </c>
@@ -13533,7 +13537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A328" s="1">
         <v>43649</v>
       </c>
@@ -13572,7 +13576,7 @@
         <v>246.3</v>
       </c>
     </row>
-    <row r="329" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A329" s="1">
         <v>43649</v>
       </c>
@@ -13611,7 +13615,7 @@
         <v>246.3</v>
       </c>
     </row>
-    <row r="330" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A330" s="1">
         <v>43649</v>
       </c>
@@ -13653,7 +13657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A331" s="1">
         <v>43649</v>
       </c>
@@ -13695,7 +13699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A332" s="1">
         <v>43649</v>
       </c>
@@ -13737,7 +13741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A333" s="1">
         <v>43649</v>
       </c>
@@ -13779,7 +13783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A334" s="1">
         <v>43649</v>
       </c>
@@ -13821,7 +13825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A335" s="1">
         <v>43649</v>
       </c>
@@ -13863,7 +13867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A336" s="1">
         <v>43649</v>
       </c>
@@ -13905,7 +13909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A337" s="1">
         <v>43649</v>
       </c>
@@ -13947,7 +13951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A338" s="1">
         <v>43649</v>
       </c>
@@ -13989,7 +13993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A339" s="1">
         <v>43649</v>
       </c>
@@ -14031,7 +14035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A340" s="1">
         <v>43649</v>
       </c>
@@ -14073,7 +14077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A341" s="1">
         <v>43649</v>
       </c>
@@ -14115,7 +14119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A342" s="1">
         <v>43649</v>
       </c>
@@ -14157,7 +14161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A343" s="1">
         <v>43649</v>
       </c>
@@ -14199,7 +14203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A344" s="1">
         <v>43649</v>
       </c>
@@ -14241,7 +14245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A345" s="1">
         <v>43649</v>
       </c>
@@ -14283,7 +14287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A346" s="1">
         <v>43649</v>
       </c>
@@ -14325,7 +14329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A347" s="1">
         <v>43649</v>
       </c>
@@ -14367,7 +14371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A348" s="1">
         <v>43649</v>
       </c>
@@ -14409,7 +14413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A349" s="1">
         <v>43649</v>
       </c>
@@ -14451,7 +14455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A350" s="1">
         <v>43649</v>
       </c>
@@ -14493,7 +14497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A351" s="1">
         <v>43649</v>
       </c>
@@ -14535,7 +14539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A352" s="1">
         <v>43649</v>
       </c>
@@ -14577,7 +14581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A353" s="1">
         <v>43649</v>
       </c>
@@ -14619,7 +14623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A354" s="1">
         <v>43649</v>
       </c>
@@ -14661,7 +14665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A355" s="1">
         <v>43649</v>
       </c>
@@ -14703,7 +14707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A356" s="1">
         <v>43649</v>
       </c>
@@ -14745,7 +14749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A357" s="1">
         <v>43649</v>
       </c>
@@ -14787,7 +14791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A358" s="1">
         <v>43649</v>
       </c>
@@ -14829,7 +14833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A359" s="1">
         <v>43649</v>
       </c>
@@ -14871,7 +14875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A360" s="1">
         <v>43649</v>
       </c>
@@ -14913,7 +14917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A361" s="1">
         <v>43649</v>
       </c>
@@ -14955,7 +14959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A362" s="1">
         <v>43649</v>
       </c>
@@ -14997,7 +15001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A363" s="1">
         <v>43649</v>
       </c>
@@ -15039,7 +15043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A364" s="1">
         <v>43649</v>
       </c>
@@ -15081,7 +15085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A365" s="1">
         <v>43649</v>
       </c>
@@ -15123,7 +15127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A366" s="1">
         <v>43649</v>
       </c>
@@ -15165,7 +15169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A367" s="1">
         <v>43649</v>
       </c>
@@ -15207,7 +15211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A368" s="1">
         <v>43649</v>
       </c>
@@ -15249,7 +15253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A369" s="1">
         <v>43649</v>
       </c>
@@ -15291,7 +15295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A370" s="1">
         <v>43649</v>
       </c>
@@ -15333,7 +15337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A371" s="1">
         <v>43649</v>
       </c>
@@ -15375,7 +15379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A372" s="1">
         <v>43649</v>
       </c>
@@ -15417,7 +15421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A373" s="1">
         <v>43649</v>
       </c>
@@ -15459,7 +15463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A374" s="1">
         <v>43649</v>
       </c>
@@ -15498,7 +15502,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="375" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A375" s="1">
         <v>43649</v>
       </c>
@@ -15537,7 +15541,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="376" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A376" s="1">
         <v>43649</v>
       </c>
@@ -15576,7 +15580,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="377" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A377" s="1">
         <v>43649</v>
       </c>
@@ -15615,7 +15619,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="378" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A378" s="1">
         <v>43649</v>
       </c>
@@ -15654,7 +15658,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="379" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A379" s="1">
         <v>43649</v>
       </c>
@@ -15693,7 +15697,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="380" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A380" s="1">
         <v>43649</v>
       </c>
@@ -15732,7 +15736,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="381" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A381" s="1">
         <v>43649</v>
       </c>
@@ -15771,7 +15775,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="382" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A382" s="1">
         <v>43649</v>
       </c>
@@ -15810,7 +15814,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="383" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A383" s="1">
         <v>43649</v>
       </c>
@@ -15849,7 +15853,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="384" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A384" s="1">
         <v>43649</v>
       </c>
@@ -15888,7 +15892,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="385" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A385" s="1">
         <v>43649</v>
       </c>
@@ -15927,7 +15931,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="386" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A386" s="1">
         <v>43649</v>
       </c>
@@ -15966,7 +15970,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="387" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A387" s="1">
         <v>43649</v>
       </c>
@@ -16005,7 +16009,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="388" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A388" s="1">
         <v>43649</v>
       </c>
@@ -16044,7 +16048,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="389" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A389" s="1">
         <v>43649</v>
       </c>
@@ -16083,7 +16087,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="390" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A390" s="1">
         <v>43649</v>
       </c>
@@ -16122,7 +16126,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="391" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A391" s="1">
         <v>43649</v>
       </c>
@@ -16161,7 +16165,7 @@
         <v>239.7</v>
       </c>
     </row>
-    <row r="392" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A392" s="1">
         <v>43649</v>
       </c>
@@ -16268,8 +16272,8 @@
         <v>244</v>
       </c>
       <c r="J394">
-        <f t="shared" ref="J394:J397" si="23">48-((16+(49/60))-(15+(8/60)))</f>
-        <v>46.316666666666663</v>
+        <f t="shared" ref="J394:J397" si="23">(48*2)-((16+(49/60))-(13+(54/60)))</f>
+        <v>93.083333333333329</v>
       </c>
       <c r="K394">
         <v>249.7</v>
@@ -16308,7 +16312,7 @@
       </c>
       <c r="J395">
         <f t="shared" si="23"/>
-        <v>46.316666666666663</v>
+        <v>93.083333333333329</v>
       </c>
       <c r="K395">
         <v>249.7</v>
@@ -16347,7 +16351,7 @@
       </c>
       <c r="J396">
         <f t="shared" si="23"/>
-        <v>46.316666666666663</v>
+        <v>93.083333333333329</v>
       </c>
       <c r="K396">
         <v>249.7</v>
@@ -16386,7 +16390,7 @@
       </c>
       <c r="J397">
         <f t="shared" si="23"/>
-        <v>46.316666666666663</v>
+        <v>93.083333333333329</v>
       </c>
       <c r="K397">
         <v>249.7</v>
@@ -16395,7 +16399,7 @@
         <v>233.89999999999998</v>
       </c>
     </row>
-    <row r="398" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A398" s="1">
         <v>43649</v>
       </c>
@@ -16434,7 +16438,7 @@
         <v>239.3</v>
       </c>
     </row>
-    <row r="399" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A399" s="1">
         <v>43649</v>
       </c>
@@ -16473,7 +16477,7 @@
         <v>239.3</v>
       </c>
     </row>
-    <row r="400" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A400" s="1">
         <v>43649</v>
       </c>
@@ -16512,7 +16516,7 @@
         <v>239.3</v>
       </c>
     </row>
-    <row r="401" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A401" s="1">
         <v>43649</v>
       </c>
@@ -16551,7 +16555,7 @@
         <v>239.3</v>
       </c>
     </row>
-    <row r="402" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A402" s="1">
         <v>43649</v>
       </c>
@@ -16590,7 +16594,7 @@
         <v>239.3</v>
       </c>
     </row>
-    <row r="403" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A403" s="1">
         <v>43649</v>
       </c>
@@ -16629,7 +16633,7 @@
         <v>239.3</v>
       </c>
     </row>
-    <row r="404" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A404" s="1">
         <v>43649</v>
       </c>
@@ -16668,7 +16672,7 @@
         <v>239.3</v>
       </c>
     </row>
-    <row r="405" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A405" s="1">
         <v>43649</v>
       </c>
@@ -16707,7 +16711,7 @@
         <v>239.3</v>
       </c>
     </row>
-    <row r="406" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A406" s="1">
         <v>43649</v>
       </c>
@@ -16746,7 +16750,7 @@
         <v>239.3</v>
       </c>
     </row>
-    <row r="407" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A407" s="1">
         <v>43649</v>
       </c>
@@ -16785,7 +16789,7 @@
         <v>239.3</v>
       </c>
     </row>
-    <row r="408" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A408" s="1">
         <v>43649</v>
       </c>
@@ -16892,8 +16896,8 @@
         <v>89</v>
       </c>
       <c r="J410">
-        <f t="shared" ref="J410:J413" si="25">48-((17+(1/60))-(15+(23/60)))</f>
-        <v>46.366666666666667</v>
+        <f t="shared" ref="J410:J413" si="25">(48*2)-((17+(1/60))-(13+(45/60)))</f>
+        <v>92.733333333333334</v>
       </c>
       <c r="K410">
         <v>249.8</v>
@@ -16932,7 +16936,7 @@
       </c>
       <c r="J411">
         <f t="shared" si="25"/>
-        <v>46.366666666666667</v>
+        <v>92.733333333333334</v>
       </c>
       <c r="K411">
         <v>249.8</v>
@@ -16971,7 +16975,7 @@
       </c>
       <c r="J412">
         <f t="shared" si="25"/>
-        <v>46.366666666666667</v>
+        <v>92.733333333333334</v>
       </c>
       <c r="K412">
         <v>249.8</v>
@@ -17010,7 +17014,7 @@
       </c>
       <c r="J413">
         <f t="shared" si="25"/>
-        <v>46.366666666666667</v>
+        <v>92.733333333333334</v>
       </c>
       <c r="K413">
         <v>249.8</v>
@@ -17019,7 +17023,7 @@
         <v>236.60000000000002</v>
       </c>
     </row>
-    <row r="414" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A414" s="1">
         <v>43649</v>
       </c>
@@ -17058,7 +17062,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="415" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A415" s="1">
         <v>43649</v>
       </c>
@@ -17097,7 +17101,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="416" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A416" s="1">
         <v>43649</v>
       </c>
@@ -17136,7 +17140,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="417" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A417" s="1">
         <v>43649</v>
       </c>
@@ -17175,7 +17179,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="418" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A418" s="1">
         <v>43649</v>
       </c>
@@ -17214,7 +17218,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="419" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A419" s="1">
         <v>43649</v>
       </c>
@@ -17253,7 +17257,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="420" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A420" s="1">
         <v>43649</v>
       </c>
@@ -17292,7 +17296,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="421" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A421" s="1">
         <v>43649</v>
       </c>
@@ -17331,7 +17335,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="422" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A422" s="1">
         <v>43649</v>
       </c>
@@ -17370,7 +17374,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="423" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A423" s="1">
         <v>43649</v>
       </c>
@@ -17409,7 +17413,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="424" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A424" s="1">
         <v>43649</v>
       </c>
@@ -17448,7 +17452,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="425" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A425" s="1">
         <v>43649</v>
       </c>
@@ -17487,7 +17491,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="426" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A426" s="1">
         <v>43649</v>
       </c>
@@ -17526,7 +17530,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="427" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A427" s="1">
         <v>43649</v>
       </c>
@@ -17565,7 +17569,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="428" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A428" s="1">
         <v>43649</v>
       </c>
@@ -17604,7 +17608,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="429" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A429" s="1">
         <v>43649</v>
       </c>
@@ -17643,7 +17647,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="430" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A430" s="1">
         <v>43649</v>
       </c>
@@ -17682,7 +17686,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="431" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A431" s="1">
         <v>43649</v>
       </c>
@@ -17721,7 +17725,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="432" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A432" s="1">
         <v>43649</v>
       </c>
@@ -17760,7 +17764,7 @@
         <v>215.7</v>
       </c>
     </row>
-    <row r="433" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A433" s="1">
         <v>43649</v>
       </c>
@@ -17799,7 +17803,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="434" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A434" s="1">
         <v>43649</v>
       </c>
@@ -17838,7 +17842,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="435" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A435" s="1">
         <v>43649</v>
       </c>
@@ -17877,7 +17881,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="436" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A436" s="1">
         <v>43649</v>
       </c>
@@ -17916,7 +17920,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="437" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A437" s="1">
         <v>43649</v>
       </c>
@@ -17955,7 +17959,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="438" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A438" s="1">
         <v>43649</v>
       </c>
@@ -17994,7 +17998,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="439" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A439" s="1">
         <v>43649</v>
       </c>
@@ -18033,7 +18037,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="440" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A440" s="1">
         <v>43649</v>
       </c>
@@ -18072,7 +18076,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="441" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A441" s="1">
         <v>43649</v>
       </c>
@@ -18111,7 +18115,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="442" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A442" s="1">
         <v>43649</v>
       </c>
@@ -18150,7 +18154,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="443" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A443" s="1">
         <v>43649</v>
       </c>
@@ -18189,7 +18193,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="444" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A444" s="1">
         <v>43649</v>
       </c>
@@ -18228,7 +18232,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="445" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A445" s="1">
         <v>43649</v>
       </c>
@@ -18267,7 +18271,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="446" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A446" s="1">
         <v>43649</v>
       </c>
@@ -18306,7 +18310,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="447" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A447" s="1">
         <v>43649</v>
       </c>
@@ -18345,7 +18349,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="448" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A448" s="1">
         <v>43649</v>
       </c>
@@ -18384,7 +18388,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="449" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A449" s="1">
         <v>43649</v>
       </c>
@@ -18423,7 +18427,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="450" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A450" s="1">
         <v>43649</v>
       </c>
@@ -18462,7 +18466,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="451" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A451" s="1">
         <v>43649</v>
       </c>
@@ -18501,7 +18505,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="452" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A452" s="1">
         <v>43649</v>
       </c>
@@ -18540,7 +18544,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="453" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A453" s="1">
         <v>43649</v>
       </c>
@@ -18579,7 +18583,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="454" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A454" s="1">
         <v>43649</v>
       </c>
@@ -18618,7 +18622,7 @@
         <v>219.6</v>
       </c>
     </row>
-    <row r="455" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A455" s="1">
         <v>43649</v>
       </c>
@@ -18660,7 +18664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="456" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A456" s="1">
         <v>43649</v>
       </c>
@@ -18702,7 +18706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="457" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A457" s="1">
         <v>43649</v>
       </c>
@@ -18858,7 +18862,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="461" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A461" s="1">
         <v>43656</v>
       </c>
@@ -18896,7 +18900,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="462" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A462" s="1">
         <v>43656</v>
       </c>
@@ -18972,7 +18976,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="464" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A464" s="1">
         <v>43656</v>
       </c>
@@ -19010,7 +19014,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="465" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A465" s="1">
         <v>43656</v>
       </c>
@@ -19048,7 +19052,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="466" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A466" s="1">
         <v>43656</v>
       </c>
@@ -19086,7 +19090,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="467" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A467" s="1">
         <v>43656</v>
       </c>
@@ -19124,7 +19128,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="468" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A468" s="1">
         <v>43656</v>
       </c>
@@ -19162,7 +19166,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="469" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A469" s="1">
         <v>43656</v>
       </c>
@@ -19200,7 +19204,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="470" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A470" s="1">
         <v>43656</v>
       </c>
@@ -19238,7 +19242,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="471" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A471" s="1">
         <v>43656</v>
       </c>
@@ -19276,7 +19280,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="472" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A472" s="1">
         <v>43656</v>
       </c>
@@ -19314,7 +19318,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="473" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A473" s="1">
         <v>43656</v>
       </c>
@@ -19352,7 +19356,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="474" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A474" s="1">
         <v>43656</v>
       </c>
@@ -19390,7 +19394,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="475" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A475" s="1">
         <v>43656</v>
       </c>
@@ -19428,7 +19432,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="476" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A476" s="1">
         <v>43656</v>
       </c>
@@ -19466,7 +19470,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="477" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A477" s="1">
         <v>43656</v>
       </c>
@@ -19504,7 +19508,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="478" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A478" s="1">
         <v>43656</v>
       </c>
@@ -19542,7 +19546,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="479" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A479" s="1">
         <v>43656</v>
       </c>
@@ -19580,7 +19584,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="480" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A480" s="1">
         <v>43656</v>
       </c>
@@ -19618,7 +19622,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="481" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A481" s="1">
         <v>43656</v>
       </c>
@@ -19656,7 +19660,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="482" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A482" s="1">
         <v>43656</v>
       </c>
@@ -19694,7 +19698,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="483" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A483" s="1">
         <v>43656</v>
       </c>
@@ -19732,7 +19736,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="484" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A484" s="1">
         <v>43656</v>
       </c>
@@ -19770,7 +19774,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="485" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A485" s="1">
         <v>43656</v>
       </c>
@@ -19808,7 +19812,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="486" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A486" s="1">
         <v>43656</v>
       </c>
@@ -19846,7 +19850,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="487" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A487" s="1">
         <v>43656</v>
       </c>
@@ -19884,7 +19888,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="488" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A488" s="1">
         <v>43656</v>
       </c>
@@ -19922,7 +19926,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="489" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A489" s="1">
         <v>43656</v>
       </c>
@@ -19960,7 +19964,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="490" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A490" s="1">
         <v>43656</v>
       </c>
@@ -19998,7 +20002,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="491" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A491" s="1">
         <v>43656</v>
       </c>
@@ -20036,7 +20040,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="492" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A492" s="1">
         <v>43656</v>
       </c>
@@ -20074,7 +20078,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="493" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A493" s="1">
         <v>43656</v>
       </c>
@@ -20112,7 +20116,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="494" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A494" s="1">
         <v>43656</v>
       </c>
@@ -20150,7 +20154,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="495" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A495" s="1">
         <v>43656</v>
       </c>
@@ -20188,7 +20192,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="496" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A496" s="1">
         <v>43656</v>
       </c>
@@ -20226,7 +20230,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="497" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A497" s="1">
         <v>43656</v>
       </c>
@@ -20264,7 +20268,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="498" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A498" s="1">
         <v>43656</v>
       </c>
@@ -20302,7 +20306,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="499" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A499" s="1">
         <v>43656</v>
       </c>
@@ -20340,7 +20344,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="500" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A500" s="1">
         <v>43656</v>
       </c>
@@ -20378,7 +20382,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="501" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A501" s="1">
         <v>43656</v>
       </c>
@@ -20416,7 +20420,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="502" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A502" s="1">
         <v>43656</v>
       </c>
@@ -20454,7 +20458,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="503" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A503" s="1">
         <v>43656</v>
       </c>
@@ -20492,7 +20496,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="504" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A504" s="1">
         <v>43656</v>
       </c>
@@ -20530,7 +20534,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="505" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A505" s="1">
         <v>43656</v>
       </c>
@@ -20568,7 +20572,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="506" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A506" s="1">
         <v>43656</v>
       </c>
@@ -20606,7 +20610,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="507" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="507" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A507" s="1">
         <v>43656</v>
       </c>
@@ -20644,7 +20648,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="508" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="508" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A508" s="1">
         <v>43656</v>
       </c>
@@ -20758,7 +20762,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="511" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="511" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A511" s="1">
         <v>43656</v>
       </c>
@@ -20796,7 +20800,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="512" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="512" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A512" s="1">
         <v>43656</v>
       </c>
@@ -20834,7 +20838,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="513" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="513" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A513" s="1">
         <v>43656</v>
       </c>
@@ -20872,7 +20876,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="514" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="514" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A514" s="1">
         <v>43656</v>
       </c>
@@ -20910,7 +20914,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="515" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="515" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A515" s="1">
         <v>43656</v>
       </c>
@@ -20948,7 +20952,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="516" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="516" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A516" s="1">
         <v>43656</v>
       </c>
@@ -20986,7 +20990,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="517" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="517" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A517" s="1">
         <v>43656</v>
       </c>
@@ -21024,7 +21028,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="518" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="518" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A518" s="1">
         <v>43656</v>
       </c>
@@ -21062,7 +21066,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="519" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="519" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A519" s="1">
         <v>43656</v>
       </c>
@@ -21100,7 +21104,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="520" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="520" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A520" s="1">
         <v>43656</v>
       </c>
@@ -21138,7 +21142,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="521" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="521" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A521" s="1">
         <v>43656</v>
       </c>
@@ -21176,7 +21180,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="522" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="522" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A522" s="1">
         <v>43656</v>
       </c>
@@ -21214,7 +21218,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="523" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="523" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A523" s="1">
         <v>43656</v>
       </c>
@@ -21252,7 +21256,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="524" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="524" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A524" s="1">
         <v>43656</v>
       </c>
@@ -21290,7 +21294,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="525" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="525" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A525" s="1">
         <v>43656</v>
       </c>
@@ -21328,7 +21332,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="526" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="526" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A526" s="1">
         <v>43656</v>
       </c>
@@ -21366,7 +21370,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="527" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="527" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A527" s="1">
         <v>43656</v>
       </c>
@@ -21404,7 +21408,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="528" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="528" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A528" s="1">
         <v>43656</v>
       </c>
@@ -21442,7 +21446,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="529" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="529" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A529" s="1">
         <v>43656</v>
       </c>
@@ -21480,7 +21484,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="530" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="530" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A530" s="1">
         <v>43656</v>
       </c>
@@ -21518,7 +21522,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="531" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="531" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A531" s="1">
         <v>43656</v>
       </c>
@@ -21556,7 +21560,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="532" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="532" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A532" s="1">
         <v>43656</v>
       </c>
@@ -21594,7 +21598,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="533" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A533" s="1">
         <v>43656</v>
       </c>
@@ -21632,7 +21636,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="534" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="534" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A534" s="1">
         <v>43656</v>
       </c>
@@ -21670,7 +21674,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="535" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="535" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A535" s="1">
         <v>43656</v>
       </c>
@@ -21708,7 +21712,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="536" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="536" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A536" s="1">
         <v>43656</v>
       </c>
@@ -21746,7 +21750,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="537" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="537" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A537" s="1">
         <v>43656</v>
       </c>
@@ -21784,7 +21788,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="538" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="538" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A538" s="1">
         <v>43656</v>
       </c>
@@ -21822,7 +21826,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="539" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="539" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A539" s="1">
         <v>43656</v>
       </c>
@@ -21860,7 +21864,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="540" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="540" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A540" s="1">
         <v>43656</v>
       </c>
@@ -21898,7 +21902,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="541" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="541" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A541" s="1">
         <v>43656</v>
       </c>
@@ -21936,7 +21940,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="542" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A542" s="1">
         <v>43656</v>
       </c>
@@ -21974,7 +21978,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="543" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="543" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A543" s="1">
         <v>43656</v>
       </c>
@@ -22012,7 +22016,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="544" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A544" s="1">
         <v>43656</v>
       </c>
@@ -22050,7 +22054,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="545" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="545" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A545" s="1">
         <v>43656</v>
       </c>
@@ -22088,7 +22092,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="546" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="546" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A546" s="1">
         <v>43656</v>
       </c>
@@ -22126,7 +22130,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="547" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="547" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A547" s="1">
         <v>43656</v>
       </c>
@@ -22164,7 +22168,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="548" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="548" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A548" s="1">
         <v>43656</v>
       </c>
@@ -22202,7 +22206,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="549" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="549" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A549" s="1">
         <v>43656</v>
       </c>
@@ -22240,7 +22244,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="550" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="550" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A550" s="1">
         <v>43656</v>
       </c>
@@ -22278,7 +22282,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="551" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="551" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A551" s="1">
         <v>43656</v>
       </c>
@@ -22316,7 +22320,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="552" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="552" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A552" s="1">
         <v>43656</v>
       </c>
@@ -22354,7 +22358,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="553" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="553" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A553" s="1">
         <v>43656</v>
       </c>
@@ -22392,7 +22396,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="554" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="554" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A554" s="1">
         <v>43656</v>
       </c>
@@ -22886,7 +22890,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="567" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="567" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A567" s="1">
         <v>43656</v>
       </c>
@@ -22924,7 +22928,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="568" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="568" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A568" s="1">
         <v>43656</v>
       </c>
@@ -22962,7 +22966,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="569" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="569" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A569" s="1">
         <v>43656</v>
       </c>
@@ -23000,7 +23004,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="570" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="570" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A570" s="1">
         <v>43656</v>
       </c>
@@ -23038,7 +23042,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="571" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="571" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A571" s="1">
         <v>43656</v>
       </c>
@@ -23076,7 +23080,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="572" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="572" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A572" s="1">
         <v>43656</v>
       </c>
@@ -23114,7 +23118,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="573" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="573" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A573" s="1">
         <v>43656</v>
       </c>
@@ -23152,7 +23156,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="574" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="574" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A574" s="1">
         <v>43656</v>
       </c>
@@ -23190,7 +23194,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="575" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="575" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A575" s="1">
         <v>43656</v>
       </c>
@@ -23228,7 +23232,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="576" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="576" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A576" s="1">
         <v>43656</v>
       </c>
@@ -23266,7 +23270,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="577" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="577" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A577" s="1">
         <v>43656</v>
       </c>
@@ -23304,7 +23308,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="578" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="578" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A578" s="1">
         <v>43656</v>
       </c>
@@ -23342,7 +23346,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="579" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="579" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A579" s="1">
         <v>43656</v>
       </c>
@@ -23380,7 +23384,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="580" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="580" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A580" s="1">
         <v>43656</v>
       </c>
@@ -23418,7 +23422,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="581" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="581" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A581" s="1">
         <v>43656</v>
       </c>
@@ -23456,7 +23460,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="582" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="582" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A582" s="1">
         <v>43656</v>
       </c>
@@ -23494,7 +23498,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="583" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="583" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A583" s="1">
         <v>43656</v>
       </c>
@@ -23532,7 +23536,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="584" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="584" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A584" s="1">
         <v>43656</v>
       </c>
@@ -23570,7 +23574,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="585" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="585" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A585" s="1">
         <v>43656</v>
       </c>
@@ -24064,7 +24068,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="598" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="598" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A598" s="1">
         <v>43656</v>
       </c>
@@ -24102,7 +24106,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="599" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="599" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A599" s="1">
         <v>43656</v>
       </c>
@@ -24140,7 +24144,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="600" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="600" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A600" s="1">
         <v>43656</v>
       </c>
@@ -24178,7 +24182,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="601" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="601" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A601" s="1">
         <v>43656</v>
       </c>
@@ -24216,7 +24220,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="602" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="602" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A602" s="1">
         <v>43656</v>
       </c>
@@ -24254,7 +24258,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="603" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="603" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A603" s="1">
         <v>43656</v>
       </c>
@@ -24292,7 +24296,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="604" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="604" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A604" s="1">
         <v>43656</v>
       </c>
@@ -24330,7 +24334,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="605" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="605" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A605" s="1">
         <v>43656</v>
       </c>
@@ -24368,7 +24372,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="606" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="606" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A606" s="1">
         <v>43656</v>
       </c>
@@ -24406,7 +24410,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="607" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="607" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A607" s="1">
         <v>43656</v>
       </c>
@@ -24444,7 +24448,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="608" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="608" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A608" s="1">
         <v>43656</v>
       </c>
@@ -24482,7 +24486,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="609" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="609" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A609" s="1">
         <v>43656</v>
       </c>
@@ -24520,7 +24524,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="610" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="610" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A610" s="1">
         <v>43656</v>
       </c>
@@ -24558,7 +24562,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="611" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="611" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A611" s="1">
         <v>43656</v>
       </c>
@@ -24596,7 +24600,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="612" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="612" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A612" s="1">
         <v>43656</v>
       </c>
@@ -24634,7 +24638,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="613" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="613" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A613" s="1">
         <v>43656</v>
       </c>
@@ -24672,7 +24676,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="614" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="614" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A614" s="1">
         <v>43656</v>
       </c>
@@ -24710,7 +24714,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="615" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="615" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A615" s="1">
         <v>43656</v>
       </c>
@@ -24748,7 +24752,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="616" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="616" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A616" s="1">
         <v>43656</v>
       </c>
@@ -24786,7 +24790,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="617" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="617" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A617" s="1">
         <v>43656</v>
       </c>
@@ -24824,7 +24828,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="618" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="618" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A618" s="1">
         <v>43656</v>
       </c>
@@ -24862,7 +24866,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="619" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="619" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A619" s="1">
         <v>43656</v>
       </c>
@@ -24901,6 +24905,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M619" xr:uid="{CE3434A0-9049-7743-890E-69C3B196F5F7}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="r"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>